<commit_message>
Switching to big endian
</commit_message>
<xml_diff>
--- a/SDE CTDB.xlsx
+++ b/SDE CTDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FRC\Stepper-Driver-Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E386425E-C56B-4F67-A6BD-B51B5FE9CC0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20651AC0-ACBF-4364-9147-BA227F6B97BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-165" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{952427E9-B5B5-44D7-A31D-EC6B3653F374}"/>
+    <workbookView xWindow="25080" yWindow="-165" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{952427E9-B5B5-44D7-A31D-EC6B3653F374}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="79">
   <si>
     <t>Opcode</t>
   </si>
@@ -225,10 +225,46 @@
     <t>Byte stuffing error</t>
   </si>
   <si>
-    <t>Reserved</t>
-  </si>
-  <si>
     <t>State</t>
+  </si>
+  <si>
+    <t>Bad version</t>
+  </si>
+  <si>
+    <t>TMC429 Status</t>
+  </si>
+  <si>
+    <t>TMC2130 Status</t>
+  </si>
+  <si>
+    <t>RESERVED</t>
+  </si>
+  <si>
+    <t>Uninit</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Left limit</t>
+  </si>
+  <si>
+    <t>Right limit</t>
+  </si>
+  <si>
+    <t>Test val</t>
+  </si>
+  <si>
+    <t>0x0201</t>
+  </si>
+  <si>
+    <t>Test Val</t>
+  </si>
+  <si>
+    <t>0x0f</t>
+  </si>
+  <si>
+    <t>0x030201</t>
   </si>
 </sst>
 </file>
@@ -264,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -282,10 +318,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,7 +646,7 @@
   <dimension ref="A1:D257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,8 +2835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6A5DC3-9274-4869-AB9F-27EC04E1BE24}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2812,20 +2854,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -2881,7 +2923,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="3">
         <v>5</v>
@@ -2903,10 +2945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A02272-D6C1-435F-80C3-C6D3E06E8CAA}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,63 +2956,72 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="9.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="3"/>
-    <col min="9" max="9" width="18.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="14.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="3"/>
-    <col min="13" max="13" width="15.42578125" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="9.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="18.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="14.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="3"/>
+    <col min="17" max="17" width="15.42578125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="O1" s="7"/>
+      <c r="P1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="6"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>5</v>
@@ -2978,446 +3029,610 @@
       <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="4">
+        <v>69</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="4">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>27</v>
+      <c r="G3" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="H3" s="4">
         <v>8</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="6">
+        <v>8</v>
+      </c>
+      <c r="K3" s="4">
+        <v>8</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="4">
+      <c r="M3" s="6">
+        <v>3</v>
+      </c>
+      <c r="N3" s="4">
         <v>8</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="4">
-        <v>2</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P3" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4">
-        <v>8</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="4">
         <v>8</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="6">
+        <v>7</v>
+      </c>
+      <c r="K4" s="4">
+        <v>8</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="4">
+      <c r="M4" s="6">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4">
         <v>24</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="R4" s="4">
+        <v>1</v>
+      </c>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4">
-        <v>8</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="4">
         <v>8</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="6">
+        <v>6</v>
+      </c>
+      <c r="K5" s="4">
+        <v>8</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="P5" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R5" s="4">
+        <v>0</v>
+      </c>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4">
+      <c r="F6" s="4"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="4">
         <v>8</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="J6" s="6">
+        <v>5</v>
+      </c>
       <c r="K6" s="4"/>
-      <c r="L6" s="4">
-        <v>24</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="6"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="F7" s="4">
+      <c r="P6" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" s="4">
+        <v>3</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+    </row>
+    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="H7" s="4">
         <v>8</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="J7" s="6">
+        <v>4</v>
+      </c>
       <c r="K7" s="4"/>
-      <c r="L7" s="4">
-        <v>24</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="6"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="P7" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R7" s="4">
+        <v>1</v>
+      </c>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+    </row>
+    <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="4">
+      <c r="F8" s="4"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="4">
         <v>8</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="J8" s="6">
+        <v>3</v>
+      </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="M8" s="6"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="P8" s="4">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+    </row>
+    <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="4">
+      <c r="F9" s="4"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="4">
         <v>8</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="J9" s="6">
+        <v>2</v>
+      </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="M9" s="6"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="P9" s="4">
+        <v>24</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+    </row>
+    <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="4">
+      <c r="F10" s="4"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="4">
         <v>8</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="J10" s="6">
+        <v>1</v>
+      </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="6"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="J11" s="6"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="6"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="6"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="J13" s="6"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="6"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="J14" s="6"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="M14" s="6"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="J15" s="6"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="M15" s="6"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="J16" s="6"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="M16" s="6"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
-    </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="J17" s="6"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="M17" s="6"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="J18" s="6"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="M18" s="6"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
-    </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="J19" s="6"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="M19" s="6"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="J20" s="6"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="M20" s="6"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
-    </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="6"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="J21" s="6"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
+      <c r="M21" s="6"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
-    </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="J22" s="6"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="M22" s="6"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-    </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="D23" s="6"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="J23" s="6"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="M23" s="6"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="P1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3425,10 +3640,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B25B54-A199-4EBC-8EAA-23B2F666D185}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3470,7 +3685,40 @@
         <v>36</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:B7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on TMC429 implementation
</commit_message>
<xml_diff>
--- a/SDE CTDB.xlsx
+++ b/SDE CTDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FRC\Stepper-Driver-Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20651AC0-ACBF-4364-9147-BA227F6B97BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B936951-2A4A-4494-BA81-84416ADB6D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-165" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{952427E9-B5B5-44D7-A31D-EC6B3653F374}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="81">
   <si>
     <t>Opcode</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>0x030201</t>
+  </si>
+  <si>
+    <t>0x060504</t>
+  </si>
+  <si>
+    <t>On Target</t>
   </si>
 </sst>
 </file>
@@ -2948,7 +2954,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3104,7 +3110,7 @@
         <v>30</v>
       </c>
       <c r="P3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>69</v>
@@ -3156,10 +3162,10 @@
         <v>1</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="R4" s="4">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
       </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
@@ -3201,10 +3207,10 @@
         <v>1</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="R5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
@@ -3236,14 +3242,14 @@
       <c r="M6" s="6"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="4">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>42</v>
+      <c r="P6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="R6" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
@@ -3269,10 +3275,10 @@
         <v>2</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="R7" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
@@ -3298,13 +3304,13 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
+      </c>
+      <c r="R8" s="4">
+        <v>1</v>
       </c>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
@@ -3333,10 +3339,10 @@
         <v>24</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>78</v>
+        <v>8</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
@@ -3361,9 +3367,15 @@
       <c r="M10" s="6"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="P10" s="4">
+        <v>24</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
     </row>

</xml_diff>

<commit_message>
Basic motor driving works!
</commit_message>
<xml_diff>
--- a/SDE CTDB.xlsx
+++ b/SDE CTDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FRC\Stepper-Driver-Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B936951-2A4A-4494-BA81-84416ADB6D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF1950F-47FD-4686-ABC6-BC436C777148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-165" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{952427E9-B5B5-44D7-A31D-EC6B3653F374}"/>
+    <workbookView xWindow="25080" yWindow="-165" windowWidth="25440" windowHeight="15390" xr2:uid="{952427E9-B5B5-44D7-A31D-EC6B3653F374}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="89">
   <si>
     <t>Opcode</t>
   </si>
@@ -159,15 +159,6 @@
     <t>Homing Status</t>
   </si>
   <si>
-    <t>Read Register</t>
-  </si>
-  <si>
-    <t>Write Register</t>
-  </si>
-  <si>
-    <t>Register Contents</t>
-  </si>
-  <si>
     <t>Communications Error Counters</t>
   </si>
   <si>
@@ -271,6 +262,39 @@
   </si>
   <si>
     <t>On Target</t>
+  </si>
+  <si>
+    <t>Read TMC429 Register</t>
+  </si>
+  <si>
+    <t>Write TMC429 Register</t>
+  </si>
+  <si>
+    <t>Read TMC2130 Register</t>
+  </si>
+  <si>
+    <t>Write TMC2130 Register</t>
+  </si>
+  <si>
+    <t>TMC429 Write Reg</t>
+  </si>
+  <si>
+    <t>TMC429 Read Reg</t>
+  </si>
+  <si>
+    <t>TMC2130 Write Reg</t>
+  </si>
+  <si>
+    <t>TMC2130 Read Reg</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>TMC429 Register Contents</t>
+  </si>
+  <si>
+    <t>TMC2130 Resister Contents</t>
   </si>
 </sst>
 </file>
@@ -306,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -322,6 +346,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -651,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15506803-107E-4CEA-AE31-1AE0D93F8418}">
   <dimension ref="A1:D257"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +697,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -684,7 +711,7 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -698,7 +725,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -712,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -723,10 +750,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -737,10 +764,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -751,10 +778,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -765,10 +792,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -782,7 +809,7 @@
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -796,7 +823,7 @@
         <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -810,7 +837,7 @@
         <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -824,7 +851,7 @@
         <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -835,10 +862,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -848,6 +875,12 @@
       <c r="B14">
         <v>12</v>
       </c>
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1854,7 +1887,7 @@
         <v>135</v>
       </c>
       <c r="C137" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -1865,7 +1898,7 @@
         <v>136</v>
       </c>
       <c r="C138" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -1875,6 +1908,9 @@
       <c r="B139">
         <v>137</v>
       </c>
+      <c r="C139" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
@@ -1883,6 +1919,9 @@
       <c r="B140">
         <v>138</v>
       </c>
+      <c r="C140" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
@@ -1891,6 +1930,9 @@
       <c r="B141">
         <v>139</v>
       </c>
+      <c r="C141" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
@@ -1899,6 +1941,9 @@
       <c r="B142">
         <v>140</v>
       </c>
+      <c r="C142" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
@@ -1907,6 +1952,9 @@
       <c r="B143">
         <v>141</v>
       </c>
+      <c r="C143" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
@@ -1915,52 +1963,43 @@
       <c r="B144">
         <v>142</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B145">
         <v>143</v>
       </c>
-      <c r="C145" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B146">
         <v>144</v>
       </c>
-      <c r="C146" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B147">
         <v>145</v>
       </c>
-      <c r="C147" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B148">
         <v>146</v>
       </c>
-      <c r="C148" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>2</v>
       </c>
@@ -1968,7 +2007,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>2</v>
       </c>
@@ -1976,7 +2015,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>2</v>
       </c>
@@ -1984,7 +2023,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>2</v>
       </c>
@@ -1992,7 +2031,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>2</v>
       </c>
@@ -2000,7 +2039,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>2</v>
       </c>
@@ -2008,7 +2047,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>2</v>
       </c>
@@ -2016,7 +2055,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>2</v>
       </c>
@@ -2024,7 +2063,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>2</v>
       </c>
@@ -2032,7 +2071,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>2</v>
       </c>
@@ -2040,7 +2079,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>2</v>
       </c>
@@ -2048,7 +2087,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>2</v>
       </c>
@@ -2839,10 +2878,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6A5DC3-9274-4869-AB9F-27EC04E1BE24}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2856,94 +2895,177 @@
     <col min="7" max="7" width="14.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="3"/>
     <col min="9" max="9" width="15.42578125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="12" width="9.140625" style="2"/>
+    <col min="13" max="13" width="11.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="2"/>
+    <col min="15" max="15" width="12.140625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="J2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="7">
+        <v>8</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="7">
+        <v>8</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="7">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="7">
         <v>8</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="H3" s="7">
+        <v>8</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="7">
+        <v>8</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="7">
+        <v>8</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="N3" s="7">
+        <v>8</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="7">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <v>24</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7">
+        <v>32</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2953,8 +3075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A02272-D6C1-435F-80C3-C6D3E06E8CAA}">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2980,35 +3102,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -3018,7 +3140,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
@@ -3027,7 +3149,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>5</v>
@@ -3036,7 +3158,7 @@
         <v>6</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>5</v>
@@ -3045,7 +3167,7 @@
         <v>6</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>5</v>
@@ -3060,7 +3182,7 @@
         <v>6</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -3071,7 +3193,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
@@ -3080,10 +3202,10 @@
         <v>8</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H3" s="4">
         <v>8</v>
@@ -3098,7 +3220,7 @@
         <v>8</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M3" s="6">
         <v>3</v>
@@ -3113,7 +3235,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="R3" s="4">
         <v>0</v>
@@ -3126,7 +3248,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
@@ -3147,7 +3269,7 @@
         <v>8</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M4" s="6">
         <v>2</v>
@@ -3162,7 +3284,7 @@
         <v>1</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="R4" s="2">
         <v>0</v>
@@ -3187,7 +3309,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J5" s="6">
         <v>6</v>
@@ -3196,7 +3318,7 @@
         <v>8</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M5" s="6">
         <v>1</v>
@@ -3207,7 +3329,7 @@
         <v>1</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="R5" s="4">
         <v>1</v>
@@ -3220,10 +3342,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -3232,7 +3354,7 @@
         <v>8</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J6" s="6">
         <v>5</v>
@@ -3246,7 +3368,7 @@
         <v>1</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="R6" s="4">
         <v>0</v>
@@ -3261,7 +3383,7 @@
         <v>8</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J7" s="6">
         <v>4</v>
@@ -3293,7 +3415,7 @@
         <v>8</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J8" s="6">
         <v>3</v>
@@ -3307,7 +3429,7 @@
         <v>2</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R8" s="4">
         <v>1</v>
@@ -3325,7 +3447,7 @@
         <v>8</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J9" s="6">
         <v>2</v>
@@ -3342,7 +3464,7 @@
         <v>8</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
@@ -3357,7 +3479,7 @@
         <v>8</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J10" s="6">
         <v>1</v>
@@ -3374,7 +3496,7 @@
         <v>7</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
@@ -3639,12 +3761,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="P1:R1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
-    <mergeCell ref="P1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3698,17 +3820,17 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="9"/>
+      <c r="A7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="10"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3716,7 +3838,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3724,7 +3846,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>